<commit_message>
Updated (and submitted) proposal peer grading
</commit_message>
<xml_diff>
--- a/Proposal_Grading_njansen_tmullins.xlsx
+++ b/Proposal_Grading_njansen_tmullins.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\643\643project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="19140" windowHeight="10845"/>
+    <workbookView xWindow="0" yWindow="138" windowWidth="19140" windowHeight="10848"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -118,6 +123,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -165,7 +173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,7 +208,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -412,16 +420,16 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="1" customWidth="1"/>
-    <col min="2" max="6" width="12.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.26171875" style="1" customWidth="1"/>
+    <col min="2" max="6" width="12.83984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +449,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -461,7 +469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -481,7 +489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -501,7 +509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -521,7 +529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -541,7 +549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -558,10 +566,10 @@
         <v>2</v>
       </c>
       <c r="F7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -581,7 +589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -613,7 +621,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -625,7 +633,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>